<commit_message>
excel data driven integration
</commit_message>
<xml_diff>
--- a/testData/Data.xlsx
+++ b/testData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0425f2fcacbf6025/Documents/VijeySurya J/Trainings/Playwright/GitRepo/demo-nopcommerce/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{EF6D8F16-3CEC-4494-92F3-AD0FAE361088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B23D6D9-4333-455D-9140-402B6CD21ECA}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{EF6D8F16-3CEC-4494-92F3-AD0FAE361088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACFD76E6-111A-4173-B4E3-58F21B5ECEE8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,10 +106,10 @@
     <t>female</t>
   </si>
   <si>
-    <t>vijeysssdaad@gmail.com</t>
-  </si>
-  <si>
-    <t>divyammmqqd@gmail.com</t>
+    <t>vijeysssdaay@gmail.com</t>
+  </si>
+  <si>
+    <t>divyammmqqy@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
argos ci integration test
</commit_message>
<xml_diff>
--- a/testData/Data.xlsx
+++ b/testData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0425f2fcacbf6025/Documents/VijeySurya J/Trainings/Playwright/GitRepo/demo-nopcommerce/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{EF6D8F16-3CEC-4494-92F3-AD0FAE361088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAE85F83-F821-470D-8CD7-AF1D7AFD3CF2}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{EF6D8F16-3CEC-4494-92F3-AD0FAE361088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31BB1DC9-B708-4EB8-8DB5-3C066FC3B2B6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,10 +106,10 @@
     <t>abc</t>
   </si>
   <si>
-    <t>divyammmqqyssuu@gmail.com</t>
-  </si>
-  <si>
-    <t>vijeysssdaayssuu@gmail.com</t>
+    <t>vijefg@gmail.com</t>
+  </si>
+  <si>
+    <t>divyfg@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +555,7 @@
         <v>1997</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
         <v>24</v>
@@ -590,7 +590,7 @@
         <v>2002</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>

</xml_diff>